<commit_message>
form diff space problem
</commit_message>
<xml_diff>
--- a/form_diff.xlsx
+++ b/form_diff.xlsx
@@ -10,7 +10,7 @@
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">工作表1!$A$1:$Y$67</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">工作表1!$A$1:$Z$67</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="390">
   <si>
     <t>deoxys (normal forme)</t>
   </si>
@@ -1550,6 +1550,26 @@
   </si>
   <si>
     <t>究极</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>alterName</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>智蛙</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>黑冰龙</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>白冰龙</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>土猫</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1779,9 +1799,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="12">
+  <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1903,7 +1925,7 @@
     <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="12">
+  <cellStyles count="14">
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="3" builtinId="9" hidden="1"/>
@@ -1915,6 +1937,8 @@
     <cellStyle name="访问过的超链接" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="513">
@@ -7888,15 +7912,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z67"/>
+  <dimension ref="A1:AA67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M52" workbookViewId="0">
-      <selection activeCell="Z67" sqref="Z67"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:27">
       <c r="A1" s="12" t="s">
         <v>16</v>
       </c>
@@ -7952,31 +7976,34 @@
         <v>33</v>
       </c>
       <c r="S1" s="12" t="s">
+        <v>385</v>
+      </c>
+      <c r="T1" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="T1" s="12" t="s">
+      <c r="U1" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="U1" s="12" t="s">
+      <c r="V1" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="V1" s="12" t="s">
+      <c r="W1" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="W1" s="12" t="s">
+      <c r="X1" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="X1" s="12" t="s">
+      <c r="Y1" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="Y1" s="12" t="s">
+      <c r="Z1" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="Z1" s="12" t="s">
+      <c r="AA1" s="12" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="42">
+    <row r="2" spans="1:27" ht="42">
       <c r="A2" s="1">
         <v>351</v>
       </c>
@@ -8033,25 +8060,28 @@
       <c r="S2" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="T2" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="U2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="V2" s="1"/>
       <c r="W2" s="1"/>
-      <c r="X2" t="s">
+      <c r="X2" s="1"/>
+      <c r="Y2" t="s">
         <v>122</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>41</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="42">
+    <row r="3" spans="1:27" ht="42">
       <c r="A3" s="1">
         <v>351</v>
       </c>
@@ -8106,27 +8136,30 @@
         <v>66</v>
       </c>
       <c r="S3" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="T3" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="V3" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="V3" s="1"/>
       <c r="W3" s="1"/>
-      <c r="X3" t="s">
+      <c r="X3" s="1"/>
+      <c r="Y3" t="s">
         <v>119</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Z3" t="s">
         <v>54</v>
       </c>
-      <c r="Z3" s="1" t="s">
+      <c r="AA3" s="1" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="42">
+    <row r="4" spans="1:27" ht="42">
       <c r="A4" s="1">
         <v>351</v>
       </c>
@@ -8181,27 +8214,30 @@
         <v>330</v>
       </c>
       <c r="S4" s="11" t="s">
+        <v>330</v>
+      </c>
+      <c r="T4" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="T4" s="1" t="s">
+      <c r="U4" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="U4" s="1" t="s">
+      <c r="V4" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="V4" s="1"/>
       <c r="W4" s="1"/>
-      <c r="X4" t="s">
+      <c r="X4" s="1"/>
+      <c r="Y4" t="s">
         <v>120</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="Z4" t="s">
         <v>55</v>
       </c>
-      <c r="Z4" s="1" t="s">
+      <c r="AA4" s="1" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="42">
+    <row r="5" spans="1:27" ht="42">
       <c r="A5" s="1">
         <v>351</v>
       </c>
@@ -8256,27 +8292,30 @@
         <v>68</v>
       </c>
       <c r="S5" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="T5" s="11" t="s">
         <v>332</v>
       </c>
-      <c r="T5" s="1" t="s">
+      <c r="U5" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="U5" s="1" t="s">
+      <c r="V5" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="V5" s="1"/>
       <c r="W5" s="1"/>
-      <c r="X5" t="s">
+      <c r="X5" s="1"/>
+      <c r="Y5" t="s">
         <v>121</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="Z5" t="s">
         <v>56</v>
       </c>
-      <c r="Z5" s="1" t="s">
+      <c r="AA5" s="1" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="43" thickBot="1">
+    <row r="6" spans="1:27" ht="43" thickBot="1">
       <c r="A6" s="1">
         <v>386</v>
       </c>
@@ -8330,28 +8369,31 @@
       <c r="R6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="S6" s="11" t="s">
+      <c r="S6" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="T6" s="11" t="s">
         <v>334</v>
       </c>
-      <c r="T6" s="1" t="s">
+      <c r="U6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="U6" s="1" t="s">
+      <c r="V6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="V6" s="1"/>
       <c r="W6" s="1"/>
-      <c r="X6" t="s">
+      <c r="X6" s="1"/>
+      <c r="Y6" t="s">
         <v>118</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="Z6" t="s">
         <v>41</v>
       </c>
-      <c r="Z6" s="1" t="s">
+      <c r="AA6" s="1" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="43" thickTop="1">
+    <row r="7" spans="1:27" ht="43" thickTop="1">
       <c r="A7" s="1">
         <v>386</v>
       </c>
@@ -8405,28 +8447,31 @@
       <c r="R7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="S7" s="12" t="s">
+      <c r="S7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="T7" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="T7" s="1" t="s">
+      <c r="U7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="U7" s="1" t="s">
+      <c r="V7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="V7" s="1"/>
       <c r="W7" s="1"/>
-      <c r="X7" t="s">
+      <c r="X7" s="1"/>
+      <c r="Y7" t="s">
         <v>117</v>
       </c>
-      <c r="Y7" t="s">
+      <c r="Z7" t="s">
         <v>42</v>
       </c>
-      <c r="Z7" s="1" t="s">
+      <c r="AA7" s="1" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="42">
+    <row r="8" spans="1:27" ht="42">
       <c r="A8" s="1">
         <v>386</v>
       </c>
@@ -8480,28 +8525,31 @@
       <c r="R8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="S8" s="12" t="s">
+      <c r="S8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="T8" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="T8" s="1" t="s">
+      <c r="U8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="U8" s="1" t="s">
+      <c r="V8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="V8" s="1"/>
       <c r="W8" s="1"/>
-      <c r="X8" t="s">
+      <c r="X8" s="1"/>
+      <c r="Y8" t="s">
         <v>116</v>
       </c>
-      <c r="Y8" t="s">
+      <c r="Z8" t="s">
         <v>43</v>
       </c>
-      <c r="Z8" s="1" t="s">
+      <c r="AA8" s="1" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="42">
+    <row r="9" spans="1:27" ht="42">
       <c r="A9" s="1">
         <v>386</v>
       </c>
@@ -8555,28 +8603,31 @@
       <c r="R9" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="S9" s="12" t="s">
+      <c r="S9" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="T9" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="T9" s="1" t="s">
+      <c r="U9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="U9" s="1" t="s">
+      <c r="V9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="V9" s="1"/>
       <c r="W9" s="1"/>
-      <c r="X9" t="s">
+      <c r="X9" s="1"/>
+      <c r="Y9" t="s">
         <v>115</v>
       </c>
-      <c r="Y9" t="s">
+      <c r="Z9" t="s">
         <v>44</v>
       </c>
-      <c r="Z9" s="1" t="s">
+      <c r="AA9" s="1" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="42">
+    <row r="10" spans="1:27" ht="42">
       <c r="A10" s="14">
         <v>413</v>
       </c>
@@ -8629,21 +8680,24 @@
       <c r="S10" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="T10" s="11"/>
+      <c r="T10" s="11" t="s">
+        <v>69</v>
+      </c>
       <c r="U10" s="11"/>
-      <c r="V10" s="1"/>
+      <c r="V10" s="11"/>
       <c r="W10" s="1"/>
-      <c r="X10" t="s">
+      <c r="X10" s="1"/>
+      <c r="Y10" t="s">
         <v>114</v>
       </c>
-      <c r="Y10" t="s">
+      <c r="Z10" t="s">
         <v>74</v>
       </c>
-      <c r="Z10" s="1" t="s">
+      <c r="AA10" s="1" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="42">
+    <row r="11" spans="1:27" ht="42">
       <c r="A11" s="14">
         <v>413</v>
       </c>
@@ -8696,19 +8750,22 @@
       <c r="S11" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="T11" s="11"/>
+      <c r="T11" s="11" t="s">
+        <v>70</v>
+      </c>
       <c r="U11" s="11"/>
-      <c r="X11" t="s">
+      <c r="V11" s="11"/>
+      <c r="Y11" t="s">
         <v>113</v>
       </c>
-      <c r="Y11" t="s">
+      <c r="Z11" t="s">
         <v>72</v>
       </c>
-      <c r="Z11" s="1" t="s">
+      <c r="AA11" s="1" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="42">
+    <row r="12" spans="1:27" ht="42">
       <c r="A12" s="14">
         <v>413</v>
       </c>
@@ -8761,19 +8818,22 @@
       <c r="S12" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="T12" s="11"/>
+      <c r="T12" s="11" t="s">
+        <v>71</v>
+      </c>
       <c r="U12" s="11"/>
-      <c r="X12" t="s">
+      <c r="V12" s="11"/>
+      <c r="Y12" t="s">
         <v>112</v>
       </c>
-      <c r="Y12" t="s">
+      <c r="Z12" t="s">
         <v>73</v>
       </c>
-      <c r="Z12" s="1" t="s">
+      <c r="AA12" s="1" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="42">
+    <row r="13" spans="1:27" ht="42">
       <c r="A13" s="14">
         <v>479</v>
       </c>
@@ -8826,19 +8886,22 @@
       <c r="S13" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="T13" s="11"/>
+      <c r="T13" s="11" t="s">
+        <v>77</v>
+      </c>
       <c r="U13" s="11"/>
-      <c r="X13" t="s">
+      <c r="V13" s="11"/>
+      <c r="Y13" t="s">
         <v>111</v>
       </c>
-      <c r="Y13" t="s">
+      <c r="Z13" t="s">
         <v>41</v>
       </c>
-      <c r="Z13" s="1" t="s">
+      <c r="AA13" s="1" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="28">
+    <row r="14" spans="1:27" ht="28">
       <c r="A14" s="14">
         <v>479</v>
       </c>
@@ -8891,19 +8954,22 @@
       <c r="S14" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="T14" s="11"/>
+      <c r="T14" s="11" t="s">
+        <v>88</v>
+      </c>
       <c r="U14" s="11"/>
-      <c r="X14" t="s">
+      <c r="V14" s="11"/>
+      <c r="Y14" t="s">
         <v>110</v>
       </c>
-      <c r="Y14" t="s">
+      <c r="Z14" t="s">
         <v>93</v>
       </c>
-      <c r="Z14" s="1" t="s">
+      <c r="AA14" s="1" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="42">
+    <row r="15" spans="1:27" ht="42">
       <c r="A15" s="14">
         <v>479</v>
       </c>
@@ -8956,19 +9022,22 @@
       <c r="S15" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="T15" s="11"/>
+      <c r="T15" s="11" t="s">
+        <v>90</v>
+      </c>
       <c r="U15" s="11"/>
-      <c r="X15" t="s">
+      <c r="V15" s="11"/>
+      <c r="Y15" t="s">
         <v>109</v>
       </c>
-      <c r="Y15" t="s">
+      <c r="Z15" t="s">
         <v>94</v>
       </c>
-      <c r="Z15" s="1" t="s">
+      <c r="AA15" s="1" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="42">
+    <row r="16" spans="1:27" ht="42">
       <c r="A16" s="14">
         <v>479</v>
       </c>
@@ -9021,19 +9090,22 @@
       <c r="S16" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="T16" s="11"/>
+      <c r="T16" s="11" t="s">
+        <v>89</v>
+      </c>
       <c r="U16" s="11"/>
-      <c r="X16" t="s">
+      <c r="V16" s="11"/>
+      <c r="Y16" t="s">
         <v>108</v>
       </c>
-      <c r="Y16" t="s">
+      <c r="Z16" t="s">
         <v>95</v>
       </c>
-      <c r="Z16" s="1" t="s">
+      <c r="AA16" s="1" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="17" spans="1:26" ht="42">
+    <row r="17" spans="1:27" ht="42">
       <c r="A17" s="14">
         <v>479</v>
       </c>
@@ -9086,19 +9158,22 @@
       <c r="S17" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="T17" s="11"/>
+      <c r="T17" s="11" t="s">
+        <v>91</v>
+      </c>
       <c r="U17" s="11"/>
-      <c r="X17" t="s">
+      <c r="V17" s="11"/>
+      <c r="Y17" t="s">
         <v>107</v>
       </c>
-      <c r="Y17" t="s">
+      <c r="Z17" t="s">
         <v>96</v>
       </c>
-      <c r="Z17" s="1" t="s">
+      <c r="AA17" s="1" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="18" spans="1:26" ht="42">
+    <row r="18" spans="1:27" ht="42">
       <c r="A18" s="14">
         <v>479</v>
       </c>
@@ -9151,19 +9226,22 @@
       <c r="S18" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="T18" s="11"/>
+      <c r="T18" s="11" t="s">
+        <v>92</v>
+      </c>
       <c r="U18" s="11"/>
-      <c r="X18" t="s">
+      <c r="V18" s="11"/>
+      <c r="Y18" t="s">
         <v>106</v>
       </c>
-      <c r="Y18" t="s">
+      <c r="Z18" t="s">
         <v>97</v>
       </c>
-      <c r="Z18" s="1" t="s">
+      <c r="AA18" s="1" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="19" spans="1:26" ht="42">
+    <row r="19" spans="1:27" ht="42">
       <c r="A19" s="14">
         <v>487</v>
       </c>
@@ -9216,19 +9294,22 @@
       <c r="S19" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="T19" s="11"/>
+      <c r="T19" s="11" t="s">
+        <v>100</v>
+      </c>
       <c r="U19" s="11"/>
-      <c r="X19" t="s">
+      <c r="V19" s="11"/>
+      <c r="Y19" t="s">
         <v>105</v>
       </c>
-      <c r="Y19" t="s">
+      <c r="Z19" t="s">
         <v>103</v>
       </c>
-      <c r="Z19" s="1" t="s">
+      <c r="AA19" s="1" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="20" spans="1:26" ht="42">
+    <row r="20" spans="1:27" ht="42">
       <c r="A20" s="14">
         <v>487</v>
       </c>
@@ -9281,19 +9362,22 @@
       <c r="S20" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="T20" s="11"/>
+      <c r="T20" s="11" t="s">
+        <v>101</v>
+      </c>
       <c r="U20" s="11"/>
-      <c r="X20" t="s">
+      <c r="V20" s="11"/>
+      <c r="Y20" t="s">
         <v>102</v>
       </c>
-      <c r="Y20" t="s">
+      <c r="Z20" t="s">
         <v>104</v>
       </c>
-      <c r="Z20" s="1" t="s">
+      <c r="AA20" s="1" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="21" spans="1:26" ht="42">
+    <row r="21" spans="1:27" ht="42">
       <c r="A21" s="14">
         <v>492</v>
       </c>
@@ -9346,19 +9430,22 @@
       <c r="S21" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="T21" s="11"/>
+      <c r="T21" s="11" t="s">
+        <v>126</v>
+      </c>
       <c r="U21" s="11"/>
-      <c r="X21" t="s">
+      <c r="V21" s="11"/>
+      <c r="Y21" t="s">
         <v>133</v>
       </c>
-      <c r="Y21" t="s">
+      <c r="Z21" t="s">
         <v>128</v>
       </c>
-      <c r="Z21" s="1" t="s">
+      <c r="AA21" s="1" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="22" spans="1:26" ht="42">
+    <row r="22" spans="1:27" ht="42">
       <c r="A22" s="14">
         <v>492</v>
       </c>
@@ -9411,19 +9498,22 @@
       <c r="S22" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="T22" s="11"/>
+      <c r="T22" s="11" t="s">
+        <v>127</v>
+      </c>
       <c r="U22" s="11"/>
-      <c r="X22" t="s">
+      <c r="V22" s="11"/>
+      <c r="Y22" t="s">
         <v>134</v>
       </c>
-      <c r="Y22" t="s">
+      <c r="Z22" t="s">
         <v>129</v>
       </c>
-      <c r="Z22" s="1" t="s">
+      <c r="AA22" s="1" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="23" spans="1:26" ht="56">
+    <row r="23" spans="1:27" ht="56">
       <c r="A23" s="14">
         <v>555</v>
       </c>
@@ -9476,19 +9566,22 @@
       <c r="S23" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="T23" s="11"/>
+      <c r="T23" s="11" t="s">
+        <v>137</v>
+      </c>
       <c r="U23" s="11"/>
-      <c r="X23" t="s">
+      <c r="V23" s="11"/>
+      <c r="Y23" t="s">
         <v>143</v>
       </c>
-      <c r="Y23" t="s">
+      <c r="Z23" t="s">
         <v>141</v>
       </c>
-      <c r="Z23" s="1" t="s">
+      <c r="AA23" s="1" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="24" spans="1:26" ht="42">
+    <row r="24" spans="1:27" ht="42">
       <c r="A24" s="14">
         <v>555</v>
       </c>
@@ -9541,19 +9634,22 @@
       <c r="S24" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="T24" s="11"/>
+      <c r="T24" s="11" t="s">
+        <v>140</v>
+      </c>
       <c r="U24" s="11"/>
-      <c r="X24" t="s">
+      <c r="V24" s="11"/>
+      <c r="Y24" t="s">
         <v>144</v>
       </c>
-      <c r="Y24" t="s">
+      <c r="Z24" t="s">
         <v>142</v>
       </c>
-      <c r="Z24" s="1" t="s">
+      <c r="AA24" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="25" spans="1:26" ht="42">
+    <row r="25" spans="1:27" ht="42">
       <c r="A25" s="14">
         <v>641</v>
       </c>
@@ -9606,19 +9702,22 @@
       <c r="S25" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="T25" s="11"/>
+      <c r="T25" s="11" t="s">
+        <v>150</v>
+      </c>
       <c r="U25" s="11"/>
-      <c r="X25" t="s">
+      <c r="V25" s="11"/>
+      <c r="Y25" t="s">
         <v>162</v>
       </c>
-      <c r="Y25" t="s">
+      <c r="Z25" t="s">
         <v>160</v>
       </c>
-      <c r="Z25" s="1" t="s">
+      <c r="AA25" s="1" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="26" spans="1:26" ht="42">
+    <row r="26" spans="1:27" ht="42">
       <c r="A26" s="14">
         <v>641</v>
       </c>
@@ -9671,19 +9770,22 @@
       <c r="S26" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="T26" s="11"/>
+      <c r="T26" s="11" t="s">
+        <v>153</v>
+      </c>
       <c r="U26" s="11"/>
-      <c r="X26" t="s">
+      <c r="V26" s="11"/>
+      <c r="Y26" t="s">
         <v>163</v>
       </c>
-      <c r="Y26" t="s">
+      <c r="Z26" t="s">
         <v>161</v>
       </c>
-      <c r="Z26" s="1" t="s">
+      <c r="AA26" s="1" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="27" spans="1:26" ht="56">
+    <row r="27" spans="1:27" ht="56">
       <c r="A27" s="14">
         <v>642</v>
       </c>
@@ -9734,21 +9836,24 @@
         <v>157</v>
       </c>
       <c r="S27" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="T27" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="T27" s="11"/>
       <c r="U27" s="11"/>
-      <c r="X27" t="s">
+      <c r="V27" s="11"/>
+      <c r="Y27" t="s">
         <v>164</v>
       </c>
-      <c r="Y27" t="s">
+      <c r="Z27" t="s">
         <v>160</v>
       </c>
-      <c r="Z27" s="1" t="s">
+      <c r="AA27" s="1" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="28" spans="1:26" ht="42">
+    <row r="28" spans="1:27" ht="42">
       <c r="A28" s="14">
         <v>642</v>
       </c>
@@ -9801,19 +9906,22 @@
       <c r="S28" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="T28" s="11"/>
+      <c r="T28" s="11" t="s">
+        <v>152</v>
+      </c>
       <c r="U28" s="11"/>
-      <c r="X28" t="s">
+      <c r="V28" s="11"/>
+      <c r="Y28" t="s">
         <v>165</v>
       </c>
-      <c r="Y28" t="s">
+      <c r="Z28" t="s">
         <v>161</v>
       </c>
-      <c r="Z28" s="1" t="s">
+      <c r="AA28" s="1" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="29" spans="1:26" ht="42">
+    <row r="29" spans="1:27" ht="42">
       <c r="A29" s="14">
         <v>645</v>
       </c>
@@ -9866,19 +9974,22 @@
       <c r="S29" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="T29" s="11"/>
+      <c r="T29" s="11" t="s">
+        <v>158</v>
+      </c>
       <c r="U29" s="11"/>
-      <c r="X29" t="s">
+      <c r="V29" s="11"/>
+      <c r="Y29" t="s">
         <v>166</v>
       </c>
-      <c r="Y29" t="s">
+      <c r="Z29" t="s">
         <v>160</v>
       </c>
-      <c r="Z29" s="1" t="s">
+      <c r="AA29" s="1" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="30" spans="1:26" ht="42">
+    <row r="30" spans="1:27" ht="42">
       <c r="A30" s="14">
         <v>645</v>
       </c>
@@ -9929,21 +10040,24 @@
         <v>159</v>
       </c>
       <c r="S30" s="11" t="s">
+        <v>389</v>
+      </c>
+      <c r="T30" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="T30" s="11"/>
       <c r="U30" s="11"/>
-      <c r="X30" t="s">
+      <c r="V30" s="11"/>
+      <c r="Y30" t="s">
         <v>167</v>
       </c>
-      <c r="Y30" t="s">
+      <c r="Z30" t="s">
         <v>161</v>
       </c>
-      <c r="Z30" s="1" t="s">
+      <c r="AA30" s="1" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="31" spans="1:26">
+    <row r="31" spans="1:27">
       <c r="A31" s="14">
         <v>646</v>
       </c>
@@ -9996,17 +10110,20 @@
       <c r="S31" s="24" t="s">
         <v>171</v>
       </c>
-      <c r="X31" t="s">
+      <c r="T31" s="24" t="s">
+        <v>171</v>
+      </c>
+      <c r="Y31" t="s">
         <v>176</v>
       </c>
-      <c r="Y31" t="s">
+      <c r="Z31" t="s">
         <v>179</v>
       </c>
-      <c r="Z31" s="1" t="s">
+      <c r="AA31" s="1" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="32" spans="1:26" ht="42">
+    <row r="32" spans="1:27" ht="42">
       <c r="A32" s="14">
         <v>646</v>
       </c>
@@ -10057,19 +10174,22 @@
         <v>174</v>
       </c>
       <c r="S32" s="11" t="s">
+        <v>388</v>
+      </c>
+      <c r="T32" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="X32" t="s">
+      <c r="Y32" t="s">
         <v>177</v>
       </c>
-      <c r="Y32" t="s">
+      <c r="Z32" t="s">
         <v>180</v>
       </c>
-      <c r="Z32" s="1" t="s">
+      <c r="AA32" s="1" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="33" spans="1:26" ht="42">
+    <row r="33" spans="1:27" ht="42">
       <c r="A33" s="14">
         <v>646</v>
       </c>
@@ -10120,19 +10240,22 @@
         <v>175</v>
       </c>
       <c r="S33" s="11" t="s">
+        <v>387</v>
+      </c>
+      <c r="T33" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="X33" t="s">
+      <c r="Y33" t="s">
         <v>178</v>
       </c>
-      <c r="Y33" t="s">
+      <c r="Z33" t="s">
         <v>181</v>
       </c>
-      <c r="Z33" s="1" t="s">
+      <c r="AA33" s="1" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="34" spans="1:26" ht="42">
+    <row r="34" spans="1:27" ht="42">
       <c r="A34" s="14">
         <v>648</v>
       </c>
@@ -10185,17 +10308,20 @@
       <c r="S34" s="24" t="s">
         <v>197</v>
       </c>
-      <c r="X34" t="s">
+      <c r="T34" s="24" t="s">
+        <v>197</v>
+      </c>
+      <c r="Y34" t="s">
         <v>196</v>
       </c>
-      <c r="Y34" t="s">
+      <c r="Z34" t="s">
         <v>194</v>
       </c>
-      <c r="Z34" s="1" t="s">
+      <c r="AA34" s="1" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="35" spans="1:26" ht="42">
+    <row r="35" spans="1:27" ht="42">
       <c r="A35" s="14">
         <v>648</v>
       </c>
@@ -10248,17 +10374,20 @@
       <c r="S35" s="24" t="s">
         <v>198</v>
       </c>
-      <c r="X35" t="s">
+      <c r="T35" s="24" t="s">
+        <v>198</v>
+      </c>
+      <c r="Y35" t="s">
         <v>326</v>
       </c>
-      <c r="Y35" t="s">
+      <c r="Z35" t="s">
         <v>195</v>
       </c>
-      <c r="Z35" s="1" t="s">
+      <c r="AA35" s="1" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="36" spans="1:26" ht="17">
+    <row r="36" spans="1:27" ht="17">
       <c r="A36" s="25">
         <v>658</v>
       </c>
@@ -10307,17 +10436,20 @@
       <c r="S36" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="X36" t="s">
+      <c r="T36" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="Y36" t="s">
         <v>188</v>
       </c>
-      <c r="Y36" t="s">
+      <c r="Z36" t="s">
         <v>179</v>
       </c>
-      <c r="Z36" s="1" t="s">
+      <c r="AA36" s="1" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="37" spans="1:26" ht="17">
+    <row r="37" spans="1:27" ht="17">
       <c r="A37" s="25">
         <v>658</v>
       </c>
@@ -10364,19 +10496,22 @@
         <v>183</v>
       </c>
       <c r="S37" s="11" t="s">
+        <v>386</v>
+      </c>
+      <c r="T37" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="X37" t="s">
+      <c r="Y37" t="s">
         <v>189</v>
       </c>
-      <c r="Y37" t="s">
+      <c r="Z37" t="s">
         <v>187</v>
       </c>
-      <c r="Z37" s="1" t="s">
+      <c r="AA37" s="1" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="38" spans="1:26" ht="42">
+    <row r="38" spans="1:27" ht="42">
       <c r="A38" s="14">
         <v>681</v>
       </c>
@@ -10429,19 +10564,22 @@
       <c r="S38" s="11" t="s">
         <v>205</v>
       </c>
-      <c r="T38" s="11"/>
+      <c r="T38" s="11" t="s">
+        <v>205</v>
+      </c>
       <c r="U38" s="11"/>
-      <c r="X38" t="s">
+      <c r="V38" s="11"/>
+      <c r="Y38" t="s">
         <v>206</v>
       </c>
-      <c r="Y38" t="s">
+      <c r="Z38" t="s">
         <v>203</v>
       </c>
-      <c r="Z38" s="1" t="s">
+      <c r="AA38" s="1" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="39" spans="1:26" ht="43" thickBot="1">
+    <row r="39" spans="1:27" ht="43" thickBot="1">
       <c r="A39" s="26">
         <v>681</v>
       </c>
@@ -10491,19 +10629,22 @@
       <c r="S39" s="11" t="s">
         <v>204</v>
       </c>
-      <c r="T39" s="11"/>
+      <c r="T39" s="11" t="s">
+        <v>204</v>
+      </c>
       <c r="U39" s="11"/>
-      <c r="X39" t="s">
+      <c r="V39" s="11"/>
+      <c r="Y39" t="s">
         <v>228</v>
       </c>
-      <c r="Y39" t="s">
+      <c r="Z39" t="s">
         <v>202</v>
       </c>
-      <c r="Z39" s="1" t="s">
+      <c r="AA39" s="1" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="40" spans="1:26" ht="43" thickTop="1">
+    <row r="40" spans="1:27" ht="43" thickTop="1">
       <c r="A40" s="14">
         <v>710</v>
       </c>
@@ -10556,17 +10697,20 @@
       <c r="S40" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="X40" t="s">
+      <c r="T40" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="Y40" t="s">
         <v>227</v>
       </c>
-      <c r="Y40" t="s">
+      <c r="Z40" t="s">
         <v>225</v>
       </c>
-      <c r="Z40" s="1" t="s">
+      <c r="AA40" s="1" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="41" spans="1:26" ht="42">
+    <row r="41" spans="1:27" ht="42">
       <c r="A41" s="14">
         <v>710</v>
       </c>
@@ -10619,17 +10763,20 @@
       <c r="S41" s="11" t="s">
         <v>217</v>
       </c>
-      <c r="X41" t="s">
+      <c r="T41" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="Y41" t="s">
         <v>227</v>
       </c>
-      <c r="Y41" t="s">
+      <c r="Z41" t="s">
         <v>226</v>
       </c>
-      <c r="Z41" s="1" t="s">
+      <c r="AA41" s="1" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="42" spans="1:26" ht="42">
+    <row r="42" spans="1:27" ht="42">
       <c r="A42" s="14">
         <v>710</v>
       </c>
@@ -10682,17 +10829,20 @@
       <c r="S42" s="11" t="s">
         <v>218</v>
       </c>
-      <c r="X42" t="s">
+      <c r="T42" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="Y42" t="s">
         <v>224</v>
       </c>
-      <c r="Y42" t="s">
+      <c r="Z42" t="s">
         <v>229</v>
       </c>
-      <c r="Z42" s="1" t="s">
+      <c r="AA42" s="1" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="43" spans="1:26" ht="42">
+    <row r="43" spans="1:27" ht="42">
       <c r="A43" s="14">
         <v>710</v>
       </c>
@@ -10745,17 +10895,20 @@
       <c r="S43" s="11" t="s">
         <v>219</v>
       </c>
-      <c r="X43" t="s">
+      <c r="T43" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="Y43" t="s">
         <v>224</v>
       </c>
-      <c r="Y43" t="s">
+      <c r="Z43" t="s">
         <v>230</v>
       </c>
-      <c r="Z43" s="1" t="s">
+      <c r="AA43" s="1" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="44" spans="1:26" ht="42">
+    <row r="44" spans="1:27" ht="42">
       <c r="A44" s="14">
         <v>711</v>
       </c>
@@ -10808,17 +10961,20 @@
       <c r="S44" s="11" t="s">
         <v>220</v>
       </c>
-      <c r="X44" t="s">
+      <c r="T44" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="Y44" t="s">
         <v>231</v>
       </c>
-      <c r="Y44" t="s">
+      <c r="Z44" t="s">
         <v>225</v>
       </c>
-      <c r="Z44" s="1" t="s">
+      <c r="AA44" s="1" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="45" spans="1:26" ht="42">
+    <row r="45" spans="1:27" ht="42">
       <c r="A45" s="14">
         <v>711</v>
       </c>
@@ -10871,17 +11027,20 @@
       <c r="S45" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="X45" t="s">
+      <c r="T45" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="Y45" t="s">
         <v>231</v>
       </c>
-      <c r="Y45" t="s">
+      <c r="Z45" t="s">
         <v>226</v>
       </c>
-      <c r="Z45" s="1" t="s">
+      <c r="AA45" s="1" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="46" spans="1:26" ht="42">
+    <row r="46" spans="1:27" ht="42">
       <c r="A46" s="14">
         <v>711</v>
       </c>
@@ -10934,17 +11093,20 @@
       <c r="S46" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="X46" t="s">
+      <c r="T46" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="Y46" t="s">
         <v>231</v>
       </c>
-      <c r="Y46" t="s">
+      <c r="Z46" t="s">
         <v>229</v>
       </c>
-      <c r="Z46" s="1" t="s">
+      <c r="AA46" s="1" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="47" spans="1:26" ht="42">
+    <row r="47" spans="1:27" ht="42">
       <c r="A47" s="14">
         <v>711</v>
       </c>
@@ -10997,17 +11159,20 @@
       <c r="S47" s="11" t="s">
         <v>223</v>
       </c>
-      <c r="X47" t="s">
+      <c r="T47" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y47" t="s">
         <v>231</v>
       </c>
-      <c r="Y47" t="s">
+      <c r="Z47" t="s">
         <v>230</v>
       </c>
-      <c r="Z47" s="1" t="s">
+      <c r="AA47" s="1" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="48" spans="1:26" ht="42">
+    <row r="48" spans="1:27" ht="42">
       <c r="A48" s="14">
         <v>718</v>
       </c>
@@ -11060,19 +11225,22 @@
       <c r="S48" s="11" t="s">
         <v>242</v>
       </c>
-      <c r="T48" s="1"/>
-      <c r="V48" s="1"/>
-      <c r="X48" t="s">
+      <c r="T48" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="U48" s="1"/>
+      <c r="W48" s="1"/>
+      <c r="Y48" t="s">
         <v>244</v>
-      </c>
-      <c r="Y48" s="35" t="s">
-        <v>322</v>
       </c>
       <c r="Z48" s="35" t="s">
         <v>322</v>
       </c>
+      <c r="AA48" s="35" t="s">
+        <v>322</v>
+      </c>
     </row>
-    <row r="49" spans="1:26" ht="42">
+    <row r="49" spans="1:27" ht="42">
       <c r="A49" s="14">
         <v>718</v>
       </c>
@@ -11125,19 +11293,22 @@
       <c r="S49" s="11" t="s">
         <v>243</v>
       </c>
-      <c r="T49" s="1"/>
-      <c r="V49" s="1"/>
-      <c r="X49" t="s">
+      <c r="T49" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="U49" s="1"/>
+      <c r="W49" s="1"/>
+      <c r="Y49" t="s">
         <v>245</v>
-      </c>
-      <c r="Y49" s="35" t="s">
-        <v>323</v>
       </c>
       <c r="Z49" s="35" t="s">
         <v>323</v>
       </c>
+      <c r="AA49" s="35" t="s">
+        <v>323</v>
+      </c>
     </row>
-    <row r="50" spans="1:26" ht="42">
+    <row r="50" spans="1:27" ht="42">
       <c r="A50" s="14">
         <v>718</v>
       </c>
@@ -11188,21 +11359,24 @@
         <v>246</v>
       </c>
       <c r="S50" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="T50" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="T50" s="1"/>
-      <c r="V50" s="1"/>
-      <c r="X50" t="s">
+      <c r="U50" s="1"/>
+      <c r="W50" s="1"/>
+      <c r="Y50" t="s">
         <v>325</v>
-      </c>
-      <c r="Y50" s="35" t="s">
-        <v>324</v>
       </c>
       <c r="Z50" s="35" t="s">
         <v>324</v>
       </c>
+      <c r="AA50" s="35" t="s">
+        <v>324</v>
+      </c>
     </row>
-    <row r="51" spans="1:26" ht="42">
+    <row r="51" spans="1:27" ht="42">
       <c r="A51" s="14">
         <v>720</v>
       </c>
@@ -11255,19 +11429,22 @@
       <c r="S51" s="11" t="s">
         <v>235</v>
       </c>
-      <c r="T51" s="11"/>
+      <c r="T51" s="11" t="s">
+        <v>235</v>
+      </c>
       <c r="U51" s="11"/>
-      <c r="X51" t="s">
+      <c r="V51" s="11"/>
+      <c r="Y51" t="s">
         <v>237</v>
       </c>
-      <c r="Y51" t="s">
+      <c r="Z51" t="s">
         <v>238</v>
       </c>
-      <c r="Z51" s="35" t="s">
+      <c r="AA51" s="35" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="52" spans="1:26" ht="42">
+    <row r="52" spans="1:27" ht="42">
       <c r="A52" s="14">
         <v>720</v>
       </c>
@@ -11320,19 +11497,22 @@
       <c r="S52" s="11" t="s">
         <v>236</v>
       </c>
-      <c r="T52" s="11"/>
+      <c r="T52" s="11" t="s">
+        <v>236</v>
+      </c>
       <c r="U52" s="11"/>
-      <c r="X52" t="s">
+      <c r="V52" s="11"/>
+      <c r="Y52" t="s">
         <v>240</v>
       </c>
-      <c r="Y52" t="s">
+      <c r="Z52" t="s">
         <v>239</v>
       </c>
-      <c r="Z52" s="35" t="s">
+      <c r="AA52" s="35" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="53" spans="1:26" ht="25">
+    <row r="53" spans="1:27" ht="25">
       <c r="A53" s="14">
         <v>741</v>
       </c>
@@ -11386,17 +11566,20 @@
       <c r="S53" s="11" t="s">
         <v>286</v>
       </c>
-      <c r="X53" t="s">
+      <c r="T53" s="11" t="s">
+        <v>286</v>
+      </c>
+      <c r="Y53" t="s">
         <v>293</v>
       </c>
-      <c r="Y53" t="s">
+      <c r="Z53" t="s">
         <v>294</v>
       </c>
-      <c r="Z53" s="35" t="s">
+      <c r="AA53" s="35" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="54" spans="1:26" ht="37">
+    <row r="54" spans="1:27" ht="37">
       <c r="A54" s="14">
         <v>741</v>
       </c>
@@ -11450,17 +11633,20 @@
       <c r="S54" s="11" t="s">
         <v>287</v>
       </c>
-      <c r="X54" t="s">
+      <c r="T54" s="11" t="s">
+        <v>287</v>
+      </c>
+      <c r="Y54" t="s">
         <v>295</v>
       </c>
-      <c r="Y54" t="s">
+      <c r="Z54" t="s">
         <v>296</v>
       </c>
-      <c r="Z54" s="35" t="s">
+      <c r="AA54" s="35" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="55" spans="1:26" ht="25">
+    <row r="55" spans="1:27" ht="25">
       <c r="A55" s="14">
         <v>741</v>
       </c>
@@ -11514,17 +11700,20 @@
       <c r="S55" s="11" t="s">
         <v>289</v>
       </c>
-      <c r="X55" t="s">
+      <c r="T55" s="11" t="s">
+        <v>289</v>
+      </c>
+      <c r="Y55" t="s">
         <v>297</v>
       </c>
-      <c r="Y55" t="s">
+      <c r="Z55" t="s">
         <v>298</v>
       </c>
-      <c r="Z55" s="35" t="s">
+      <c r="AA55" s="35" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="56" spans="1:26" ht="37">
+    <row r="56" spans="1:27" ht="37">
       <c r="A56" s="14">
         <v>741</v>
       </c>
@@ -11578,17 +11767,20 @@
       <c r="S56" s="11" t="s">
         <v>288</v>
       </c>
-      <c r="X56" t="s">
+      <c r="T56" s="11" t="s">
+        <v>288</v>
+      </c>
+      <c r="Y56" t="s">
         <v>299</v>
       </c>
-      <c r="Y56" t="s">
+      <c r="Z56" t="s">
         <v>300</v>
       </c>
-      <c r="Z56" s="35" t="s">
+      <c r="AA56" s="35" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="57" spans="1:26" ht="37">
+    <row r="57" spans="1:27" ht="37">
       <c r="A57" s="14">
         <v>745</v>
       </c>
@@ -11642,17 +11834,20 @@
       <c r="S57" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="X57" t="s">
+      <c r="T57" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="Y57" t="s">
         <v>257</v>
       </c>
-      <c r="Y57" t="s">
+      <c r="Z57" t="s">
         <v>258</v>
       </c>
-      <c r="Z57" s="35" t="s">
+      <c r="AA57" s="35" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="58" spans="1:26" ht="37">
+    <row r="58" spans="1:27" ht="37">
       <c r="A58" s="14">
         <v>745</v>
       </c>
@@ -11706,17 +11901,20 @@
       <c r="S58" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="X58" t="s">
+      <c r="T58" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="Y58" t="s">
         <v>263</v>
       </c>
-      <c r="Y58" t="s">
+      <c r="Z58" t="s">
         <v>259</v>
       </c>
-      <c r="Z58" s="35" t="s">
+      <c r="AA58" s="35" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="59" spans="1:26" ht="25">
+    <row r="59" spans="1:27" ht="25">
       <c r="A59" s="14">
         <v>745</v>
       </c>
@@ -11770,17 +11968,20 @@
       <c r="S59" s="11" t="s">
         <v>256</v>
       </c>
-      <c r="X59" t="s">
+      <c r="T59" s="11" t="s">
+        <v>256</v>
+      </c>
+      <c r="Y59" t="s">
         <v>264</v>
       </c>
-      <c r="Y59" t="s">
+      <c r="Z59" t="s">
         <v>260</v>
       </c>
-      <c r="Z59" s="35" t="s">
+      <c r="AA59" s="35" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="60" spans="1:26" ht="25">
+    <row r="60" spans="1:27" ht="25">
       <c r="A60" s="14">
         <v>746</v>
       </c>
@@ -11834,17 +12035,20 @@
       <c r="S60" s="11" t="s">
         <v>309</v>
       </c>
-      <c r="X60" t="s">
+      <c r="T60" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="Y60" t="s">
         <v>265</v>
       </c>
-      <c r="Y60" t="s">
+      <c r="Z60" t="s">
         <v>261</v>
       </c>
-      <c r="Z60" s="35" t="s">
+      <c r="AA60" s="35" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="61" spans="1:26" ht="25">
+    <row r="61" spans="1:27" ht="25">
       <c r="A61" s="14">
         <v>746</v>
       </c>
@@ -11898,17 +12102,20 @@
       <c r="S61" s="11" t="s">
         <v>310</v>
       </c>
-      <c r="X61" t="s">
+      <c r="T61" s="11" t="s">
+        <v>310</v>
+      </c>
+      <c r="Y61" t="s">
         <v>266</v>
       </c>
-      <c r="Y61" t="s">
+      <c r="Z61" t="s">
         <v>262</v>
       </c>
-      <c r="Z61" s="35" t="s">
+      <c r="AA61" s="35" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="62" spans="1:26" ht="37">
+    <row r="62" spans="1:27" ht="37">
       <c r="A62" s="14">
         <v>774</v>
       </c>
@@ -11962,17 +12169,20 @@
       <c r="S62" s="11" t="s">
         <v>268</v>
       </c>
-      <c r="X62" t="s">
+      <c r="T62" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="Y62" t="s">
         <v>270</v>
       </c>
-      <c r="Y62" t="s">
+      <c r="Z62" t="s">
         <v>271</v>
       </c>
-      <c r="Z62" s="35" t="s">
+      <c r="AA62" s="35" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="63" spans="1:26" ht="25">
+    <row r="63" spans="1:27" ht="25">
       <c r="A63" s="14">
         <v>774</v>
       </c>
@@ -12026,17 +12236,20 @@
       <c r="S63" s="11" t="s">
         <v>269</v>
       </c>
-      <c r="X63" t="s">
+      <c r="T63" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="Y63" t="s">
         <v>273</v>
       </c>
-      <c r="Y63" t="s">
+      <c r="Z63" t="s">
         <v>272</v>
       </c>
-      <c r="Z63" s="35" t="s">
+      <c r="AA63" s="35" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="64" spans="1:26">
+    <row r="64" spans="1:27">
       <c r="A64" s="14">
         <v>800</v>
       </c>
@@ -12090,17 +12303,20 @@
       <c r="S64" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="X64" t="s">
+      <c r="T64" s="11" t="s">
+        <v>302</v>
+      </c>
+      <c r="Y64" t="s">
         <v>317</v>
       </c>
-      <c r="Y64" t="s">
+      <c r="Z64" t="s">
         <v>179</v>
       </c>
-      <c r="Z64" s="35" t="s">
+      <c r="AA64" s="35" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="65" spans="1:26" ht="25">
+    <row r="65" spans="1:27" ht="25">
       <c r="A65" s="14">
         <v>800</v>
       </c>
@@ -12154,17 +12370,20 @@
       <c r="S65" s="11" t="s">
         <v>306</v>
       </c>
-      <c r="X65" t="s">
+      <c r="T65" s="11" t="s">
+        <v>306</v>
+      </c>
+      <c r="Y65" t="s">
         <v>318</v>
       </c>
-      <c r="Y65" t="s">
+      <c r="Z65" t="s">
         <v>314</v>
       </c>
-      <c r="Z65" s="35" t="s">
+      <c r="AA65" s="35" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="66" spans="1:26">
+    <row r="66" spans="1:27">
       <c r="A66" s="14">
         <v>800</v>
       </c>
@@ -12218,17 +12437,20 @@
       <c r="S66" s="11" t="s">
         <v>307</v>
       </c>
-      <c r="X66" t="s">
+      <c r="T66" s="11" t="s">
+        <v>307</v>
+      </c>
+      <c r="Y66" t="s">
         <v>319</v>
       </c>
-      <c r="Y66" t="s">
+      <c r="Z66" t="s">
         <v>315</v>
       </c>
-      <c r="Z66" s="35" t="s">
+      <c r="AA66" s="35" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="67" spans="1:26">
+    <row r="67" spans="1:27">
       <c r="A67" s="14">
         <v>800</v>
       </c>
@@ -12282,13 +12504,16 @@
       <c r="S67" s="11" t="s">
         <v>308</v>
       </c>
-      <c r="X67" t="s">
+      <c r="T67" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="Y67" t="s">
         <v>320</v>
       </c>
-      <c r="Y67" t="s">
+      <c r="Z67" t="s">
         <v>316</v>
       </c>
-      <c r="Z67" s="35" t="s">
+      <c r="AA67" s="35" t="s">
         <v>384</v>
       </c>
     </row>
@@ -14870,9 +15095,9 @@
     <hyperlink ref="R10" r:id="rId8" tooltip="结草贵妇" display="结草贵妇"/>
     <hyperlink ref="R12" r:id="rId9" tooltip="结草贵妇" display="结草贵妇"/>
     <hyperlink ref="R11" r:id="rId10" tooltip="结草贵妇" display="结草贵妇"/>
-    <hyperlink ref="S10" r:id="rId11" tooltip="结草贵妇" display="结草贵妇"/>
-    <hyperlink ref="S12" r:id="rId12" tooltip="结草贵妇" display="结草贵妇"/>
-    <hyperlink ref="S11" r:id="rId13" tooltip="结草贵妇" display="结草贵妇"/>
+    <hyperlink ref="T10" r:id="rId11" tooltip="结草贵妇" display="结草贵妇"/>
+    <hyperlink ref="T12" r:id="rId12" tooltip="结草贵妇" display="结草贵妇"/>
+    <hyperlink ref="T11" r:id="rId13" tooltip="结草贵妇" display="结草贵妇"/>
     <hyperlink ref="B14" r:id="rId14" tooltip="Rotom (Pokémon)" display="http://bulbapedia.bulbagarden.net/wiki/Rotom_(Pok%C3%A9mon)"/>
     <hyperlink ref="L13:L18" r:id="rId15" tooltip="Psychic (type)" display="https://bulbapedia.bulbagarden.net/wiki/Psychic_(type)"/>
     <hyperlink ref="B13" r:id="rId16" tooltip="Rotom (Pokémon)" display="http://bulbapedia.bulbagarden.net/wiki/Rotom_(Pok%C3%A9mon)"/>
@@ -14886,32 +15111,32 @@
     <hyperlink ref="R16" r:id="rId24" tooltip="洛托姆" display="洛托姆"/>
     <hyperlink ref="R17" r:id="rId25" tooltip="洛托姆" display="洛托姆"/>
     <hyperlink ref="R18" r:id="rId26" tooltip="洛托姆" display="洛托姆"/>
-    <hyperlink ref="S13" r:id="rId27" tooltip="洛托姆"/>
-    <hyperlink ref="S14" r:id="rId28" tooltip="洛托姆" display="洛托姆"/>
-    <hyperlink ref="S15" r:id="rId29" tooltip="洛托姆" display="洛托姆"/>
-    <hyperlink ref="S16" r:id="rId30" tooltip="洛托姆" display="洛托姆"/>
-    <hyperlink ref="S17" r:id="rId31" tooltip="洛托姆" display="洛托姆"/>
-    <hyperlink ref="S18" r:id="rId32" tooltip="洛托姆" display="洛托姆"/>
+    <hyperlink ref="T13" r:id="rId27" tooltip="洛托姆"/>
+    <hyperlink ref="T14" r:id="rId28" tooltip="洛托姆" display="洛托姆"/>
+    <hyperlink ref="T15" r:id="rId29" tooltip="洛托姆" display="洛托姆"/>
+    <hyperlink ref="T16" r:id="rId30" tooltip="洛托姆" display="洛托姆"/>
+    <hyperlink ref="T17" r:id="rId31" tooltip="洛托姆" display="洛托姆"/>
+    <hyperlink ref="T18" r:id="rId32" tooltip="洛托姆" display="洛托姆"/>
     <hyperlink ref="B19" r:id="rId33" tooltip="Giratina (Pokémon)" display="http://bulbapedia.bulbagarden.net/wiki/Giratina_(Pok%C3%A9mon)"/>
     <hyperlink ref="B20" r:id="rId34" tooltip="Giratina (Pokémon)" display="http://bulbapedia.bulbagarden.net/wiki/Giratina_(Pok%C3%A9mon)"/>
     <hyperlink ref="L19:L20" r:id="rId35" tooltip="Psychic (type)" display="https://bulbapedia.bulbagarden.net/wiki/Psychic_(type)"/>
     <hyperlink ref="R19" r:id="rId36" tooltip="黑夜魔灵" display="黑夜魔灵"/>
     <hyperlink ref="R20" r:id="rId37" tooltip="冰伊布" display="冰伊布"/>
-    <hyperlink ref="S19" r:id="rId38" tooltip="黑夜魔灵" display="黑夜魔灵"/>
-    <hyperlink ref="S20" r:id="rId39" tooltip="冰伊布" display="冰伊布"/>
+    <hyperlink ref="T19" r:id="rId38" tooltip="黑夜魔灵" display="黑夜魔灵"/>
+    <hyperlink ref="T20" r:id="rId39" tooltip="冰伊布" display="冰伊布"/>
     <hyperlink ref="B22" r:id="rId40" tooltip="Shaymin (Pokémon)" display="http://bulbapedia.bulbagarden.net/wiki/Shaymin_(Pok%C3%A9mon)"/>
     <hyperlink ref="B21" r:id="rId41" tooltip="Shaymin (Pokémon)" display="http://bulbapedia.bulbagarden.net/wiki/Shaymin_(Pok%C3%A9mon)"/>
     <hyperlink ref="L21:L22" r:id="rId42" tooltip="Psychic (type)" display="https://bulbapedia.bulbagarden.net/wiki/Psychic_(type)"/>
     <hyperlink ref="R21" r:id="rId43" tooltip="大朝北鼻" display="大朝北鼻"/>
     <hyperlink ref="R22" r:id="rId44" tooltip="艾路雷朵" display="艾路雷朵"/>
-    <hyperlink ref="S21" r:id="rId45" tooltip="大朝北鼻" display="大朝北鼻"/>
-    <hyperlink ref="S22" r:id="rId46" tooltip="艾路雷朵" display="艾路雷朵"/>
+    <hyperlink ref="T21" r:id="rId45" tooltip="大朝北鼻" display="大朝北鼻"/>
+    <hyperlink ref="T22" r:id="rId46" tooltip="艾路雷朵" display="艾路雷朵"/>
     <hyperlink ref="L23:L24" r:id="rId47" tooltip="Psychic (type)" display="https://bulbapedia.bulbagarden.net/wiki/Psychic_(type)"/>
     <hyperlink ref="B24" r:id="rId48" tooltip="Darmanitan (Pokémon)" display="http://bulbapedia.bulbagarden.net/wiki/Darmanitan_(Pok%C3%A9mon)"/>
     <hyperlink ref="L24" r:id="rId49" tooltip="Psychic (type)" display="https://bulbapedia.bulbagarden.net/wiki/Psychic_(type)"/>
     <hyperlink ref="L23" r:id="rId50" tooltip="Psychic (type)" display="https://bulbapedia.bulbagarden.net/wiki/Psychic_(type)"/>
     <hyperlink ref="B23" r:id="rId51" tooltip="Darmanitan (Pokémon)" display="http://bulbapedia.bulbagarden.net/wiki/Darmanitan_(Pok%C3%A9mon)"/>
-    <hyperlink ref="S23" r:id="rId52" tooltip="达摩狒狒"/>
+    <hyperlink ref="T23" r:id="rId52" tooltip="达摩狒狒"/>
     <hyperlink ref="R23" r:id="rId53" tooltip="达摩狒狒"/>
     <hyperlink ref="B26" r:id="rId54" tooltip="Tornadus (Pokémon)" display="http://bulbapedia.bulbagarden.net/wiki/Tornadus_(Pok%C3%A9mon)"/>
     <hyperlink ref="B25" r:id="rId55" tooltip="Tornadus (Pokémon)" display="http://bulbapedia.bulbagarden.net/wiki/Tornadus_(Pok%C3%A9mon)"/>
@@ -14969,7 +15194,22 @@
     <hyperlink ref="L66" r:id="rId107" tooltip="Psychic (type)" display="https://bulbapedia.bulbagarden.net/wiki/Psychic_(type)"/>
     <hyperlink ref="L67" r:id="rId108" tooltip="Psychic (type)" display="https://bulbapedia.bulbagarden.net/wiki/Psychic_(type)"/>
     <hyperlink ref="R67" r:id="rId109" location=".E5.A5.88.E5.85.8B.E6.B4.9B.E5.85.B9.E7.8E.9B" tooltip="形态差异"/>
-    <hyperlink ref="S67" r:id="rId110" location=".E5.A5.88.E5.85.8B.E6.B4.9B.E5.85.B9.E7.8E.9B" tooltip="形态差异"/>
+    <hyperlink ref="T67" r:id="rId110" location=".E5.A5.88.E5.85.8B.E6.B4.9B.E5.85.B9.E7.8E.9B" tooltip="形态差异"/>
+    <hyperlink ref="S10" r:id="rId111" tooltip="结草贵妇" display="结草贵妇"/>
+    <hyperlink ref="S12" r:id="rId112" tooltip="结草贵妇" display="结草贵妇"/>
+    <hyperlink ref="S11" r:id="rId113" tooltip="结草贵妇" display="结草贵妇"/>
+    <hyperlink ref="S13" r:id="rId114" tooltip="洛托姆"/>
+    <hyperlink ref="S14" r:id="rId115" tooltip="洛托姆" display="洛托姆"/>
+    <hyperlink ref="S15" r:id="rId116" tooltip="洛托姆" display="洛托姆"/>
+    <hyperlink ref="S16" r:id="rId117" tooltip="洛托姆" display="洛托姆"/>
+    <hyperlink ref="S17" r:id="rId118" tooltip="洛托姆" display="洛托姆"/>
+    <hyperlink ref="S18" r:id="rId119" tooltip="洛托姆" display="洛托姆"/>
+    <hyperlink ref="S19" r:id="rId120" tooltip="黑夜魔灵" display="黑夜魔灵"/>
+    <hyperlink ref="S20" r:id="rId121" tooltip="冰伊布" display="冰伊布"/>
+    <hyperlink ref="S21" r:id="rId122" tooltip="大朝北鼻" display="大朝北鼻"/>
+    <hyperlink ref="S22" r:id="rId123" tooltip="艾路雷朵" display="艾路雷朵"/>
+    <hyperlink ref="S23" r:id="rId124" tooltip="达摩狒狒"/>
+    <hyperlink ref="S67" r:id="rId125" location=".E5.A5.88.E5.85.8B.E6.B4.9B.E5.85.B9.E7.8E.9B" tooltip="形态差异"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
+alter name for mega/diff form
</commit_message>
<xml_diff>
--- a/form_diff.xlsx
+++ b/form_diff.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="395">
   <si>
     <t>deoxys (normal forme)</t>
   </si>
@@ -1570,6 +1570,26 @@
   </si>
   <si>
     <t>土猫</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>微波炉</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>洗衣机</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>冰箱</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>电风扇</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>割草机</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -7914,8 +7934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8952,7 +8972,7 @@
         <v>88</v>
       </c>
       <c r="S14" s="11" t="s">
-        <v>88</v>
+        <v>390</v>
       </c>
       <c r="T14" s="11" t="s">
         <v>88</v>
@@ -9020,7 +9040,7 @@
         <v>90</v>
       </c>
       <c r="S15" s="11" t="s">
-        <v>90</v>
+        <v>391</v>
       </c>
       <c r="T15" s="11" t="s">
         <v>90</v>
@@ -9088,7 +9108,7 @@
         <v>89</v>
       </c>
       <c r="S16" s="11" t="s">
-        <v>89</v>
+        <v>392</v>
       </c>
       <c r="T16" s="11" t="s">
         <v>89</v>
@@ -9156,7 +9176,7 @@
         <v>91</v>
       </c>
       <c r="S17" s="11" t="s">
-        <v>91</v>
+        <v>393</v>
       </c>
       <c r="T17" s="11" t="s">
         <v>91</v>
@@ -9224,7 +9244,7 @@
         <v>92</v>
       </c>
       <c r="S18" s="11" t="s">
-        <v>92</v>
+        <v>394</v>
       </c>
       <c r="T18" s="11" t="s">
         <v>92</v>

</xml_diff>

<commit_message>
moveset string function modified for pokemon with different forms
</commit_message>
<xml_diff>
--- a/form_diff.xlsx
+++ b/form_diff.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="412">
   <si>
     <t>deoxys (normal forme)</t>
   </si>
@@ -241,19 +241,7 @@
     <t xml:space="preserve"> Normal</t>
   </si>
   <si>
-    <t>'Bite(--)Rock Smash(--)'</t>
-  </si>
-  <si>
-    <t>'Ancient Power(--)Crunch(--)Stomp(--)'</t>
-  </si>
-  <si>
     <t>飘浮泡泡</t>
-  </si>
-  <si>
-    <t>4,16,</t>
-  </si>
-  <si>
-    <t>98,8,82,</t>
   </si>
   <si>
     <t xml:space="preserve"> Fire</t>
@@ -1604,12 +1592,73 @@
     <t>土地云(化身形态)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>Tackle(--)Hex(--)'</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tackle(--)Ember(--)'</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tackle(--)Water Gun(--)'</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hurricane(--)Energy Ball(--)'</t>
+  </si>
+  <si>
+    <t>Fire Blast(--)Solar Beam(--)'</t>
+  </si>
+  <si>
+    <t>Hydro Pump(--)Thunder(--)'</t>
+  </si>
+  <si>
+    <t>Counter(--)Zen Headbutt(--)'</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Psycho Boost(--)Swift(--)Zap Cannon(--)'</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tackle(--)Powder Snow(--)'</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Blizzard(--)Ice Beam(--)'</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>36,27,</t>
+  </si>
+  <si>
+    <t>36,18,</t>
+  </si>
+  <si>
+    <t>36,56,</t>
+  </si>
+  <si>
+    <t>36,35,</t>
+  </si>
+  <si>
+    <t>43,57,</t>
+  </si>
+  <si>
+    <t>34,53,</t>
+  </si>
+  <si>
+    <t>108,13,</t>
+  </si>
+  <si>
+    <t>72,68,</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1696,6 +1745,14 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="15">
@@ -1831,7 +1888,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="14">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1846,8 +1903,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1956,8 +2014,10 @@
     <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="14">
+  <cellStyles count="15">
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="3" builtinId="9" hidden="1"/>
@@ -1971,6 +2031,7 @@
     <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="513">
@@ -7946,8 +8007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L23" workbookViewId="0">
-      <selection activeCell="W29" sqref="W29"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8008,7 +8069,7 @@
         <v>33</v>
       </c>
       <c r="S1" s="12" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="T1" s="12" t="s">
         <v>34</v>
@@ -8032,7 +8093,7 @@
         <v>40</v>
       </c>
       <c r="AA1" s="12" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="2" spans="1:27" ht="42">
@@ -8040,7 +8101,7 @@
         <v>351</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C2" s="3">
         <v>70</v>
@@ -8078,39 +8139,39 @@
       <c r="M2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>47</v>
+      <c r="N2" s="46" t="s">
+        <v>394</v>
+      </c>
+      <c r="O2" s="47" t="s">
+        <v>397</v>
       </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S2" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="T2" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>49</v>
+        <v>404</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>50</v>
+        <v>408</v>
       </c>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
       <c r="Y2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="Z2" t="s">
         <v>41</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="42">
@@ -8118,7 +8179,7 @@
         <v>351</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C3" s="3">
         <v>70</v>
@@ -8154,41 +8215,41 @@
         <v>139</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="O3" s="1" t="s">
         <v>47</v>
+      </c>
+      <c r="N3" s="46" t="s">
+        <v>395</v>
+      </c>
+      <c r="O3" s="47" t="s">
+        <v>398</v>
       </c>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="11" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="S3" s="11" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="T3" s="11" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>49</v>
+        <v>405</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>50</v>
+        <v>409</v>
       </c>
       <c r="W3" s="1"/>
       <c r="X3" s="1"/>
       <c r="Y3" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="Z3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="AA3" s="1" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="42">
@@ -8196,7 +8257,7 @@
         <v>351</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C4" s="3">
         <v>70</v>
@@ -8232,41 +8293,41 @@
         <v>139</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="N4" s="46" t="s">
+        <v>396</v>
+      </c>
+      <c r="O4" s="47" t="s">
+        <v>399</v>
       </c>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="11" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="S4" s="11" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="T4" s="11" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>49</v>
+        <v>406</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>50</v>
+        <v>410</v>
       </c>
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
       <c r="Y4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="Z4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="AA4" s="1" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="42">
@@ -8274,7 +8335,7 @@
         <v>351</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C5" s="3">
         <v>70</v>
@@ -8310,41 +8371,41 @@
         <v>139</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
+      </c>
+      <c r="N5" s="46" t="s">
+        <v>402</v>
+      </c>
+      <c r="O5" s="46" t="s">
+        <v>403</v>
       </c>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="11" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="S5" s="11" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="T5" s="11" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>49</v>
+        <v>407</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>50</v>
+        <v>411</v>
       </c>
       <c r="W5" s="1"/>
       <c r="X5" s="1"/>
       <c r="Y5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="Z5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="AA5" s="1" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="43" thickBot="1">
@@ -8390,11 +8451,11 @@
       <c r="M6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="N6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>3</v>
+      <c r="N6" s="46" t="s">
+        <v>400</v>
+      </c>
+      <c r="O6" s="46" t="s">
+        <v>401</v>
       </c>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
@@ -8405,7 +8466,7 @@
         <v>4</v>
       </c>
       <c r="T6" s="11" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="U6" s="1" t="s">
         <v>5</v>
@@ -8416,13 +8477,13 @@
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
       <c r="Y6" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="Z6" t="s">
         <v>41</v>
       </c>
       <c r="AA6" s="1" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="43" thickTop="1">
@@ -8477,7 +8538,7 @@
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="S7" s="1" t="s">
         <v>8</v>
@@ -8494,13 +8555,13 @@
       <c r="W7" s="1"/>
       <c r="X7" s="1"/>
       <c r="Y7" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="Z7" t="s">
         <v>42</v>
       </c>
       <c r="AA7" s="1" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="42">
@@ -8555,7 +8616,7 @@
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="S8" s="1" t="s">
         <v>12</v>
@@ -8572,13 +8633,13 @@
       <c r="W8" s="1"/>
       <c r="X8" s="1"/>
       <c r="Y8" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="Z8" t="s">
         <v>43</v>
       </c>
       <c r="AA8" s="1" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="42">
@@ -8633,10 +8694,10 @@
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="S9" s="1" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="T9" s="12" t="s">
         <v>15</v>
@@ -8650,13 +8711,13 @@
       <c r="W9" s="1"/>
       <c r="X9" s="1"/>
       <c r="Y9" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="Z9" t="s">
         <v>44</v>
       </c>
       <c r="AA9" s="1" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="42">
@@ -8664,7 +8725,7 @@
         <v>413</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C10" s="3">
         <v>60</v>
@@ -8700,33 +8761,33 @@
         <v>189</v>
       </c>
       <c r="M10" s="12" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="11" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="S10" s="11" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="T10" s="11" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="U10" s="11"/>
       <c r="V10" s="11"/>
       <c r="W10" s="1"/>
       <c r="X10" s="1"/>
       <c r="Y10" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="Z10" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="AA10" s="1" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="42">
@@ -8734,7 +8795,7 @@
         <v>413</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C11" s="3">
         <v>60</v>
@@ -8770,31 +8831,31 @@
         <v>189</v>
       </c>
       <c r="M11" s="12" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
       <c r="R11" s="11" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="S11" s="11" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="T11" s="11" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="U11" s="11"/>
       <c r="V11" s="11"/>
       <c r="Y11" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="Z11" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="AA11" s="1" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="42">
@@ -8802,7 +8863,7 @@
         <v>413</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C12" s="3">
         <v>60</v>
@@ -8838,31 +8899,31 @@
         <v>175</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="11" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="S12" s="11" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="T12" s="11" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="U12" s="11"/>
       <c r="V12" s="11"/>
       <c r="Y12" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="Z12" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="AA12" s="1" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="13" spans="1:27" ht="42">
@@ -8870,7 +8931,7 @@
         <v>479</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C13" s="3">
         <v>50</v>
@@ -8906,31 +8967,31 @@
         <v>159</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="11" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="S13" s="11" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="T13" s="11" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="U13" s="11"/>
       <c r="V13" s="11"/>
       <c r="Y13" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="Z13" t="s">
         <v>41</v>
       </c>
       <c r="AA13" s="1" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="14" spans="1:27" ht="28">
@@ -8938,7 +8999,7 @@
         <v>479</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C14" s="3">
         <v>50</v>
@@ -8974,31 +9035,31 @@
         <v>219</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
       <c r="R14" s="11" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="S14" s="11" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="T14" s="11" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="U14" s="11"/>
       <c r="V14" s="11"/>
       <c r="Y14" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="Z14" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="AA14" s="1" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="42">
@@ -9006,7 +9067,7 @@
         <v>479</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C15" s="3">
         <v>50</v>
@@ -9042,31 +9103,31 @@
         <v>219</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="11" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="S15" s="11" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="T15" s="11" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="U15" s="11"/>
       <c r="V15" s="11"/>
       <c r="Y15" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="Z15" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="AA15" s="1" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="16" spans="1:27" ht="42">
@@ -9074,7 +9135,7 @@
         <v>479</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C16" s="3">
         <v>50</v>
@@ -9110,31 +9171,31 @@
         <v>219</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
       <c r="R16" s="11" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="S16" s="11" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="T16" s="11" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="U16" s="11"/>
       <c r="V16" s="11"/>
       <c r="Y16" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="Z16" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="AA16" s="1" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="17" spans="1:27" ht="42">
@@ -9142,7 +9203,7 @@
         <v>479</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C17" s="3">
         <v>50</v>
@@ -9178,31 +9239,31 @@
         <v>219</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="11" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="S17" s="11" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="T17" s="11" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="U17" s="11"/>
       <c r="V17" s="11"/>
       <c r="Y17" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="Z17" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="AA17" s="1" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="18" spans="1:27" ht="42">
@@ -9210,7 +9271,7 @@
         <v>479</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C18" s="3">
         <v>50</v>
@@ -9246,31 +9307,31 @@
         <v>159</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="11" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="S18" s="11" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="T18" s="11" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="U18" s="11"/>
       <c r="V18" s="11"/>
       <c r="Y18" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="Z18" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="AA18" s="1" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="19" spans="1:27" ht="42">
@@ -9278,7 +9339,7 @@
         <v>487</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C19" s="3">
         <v>150</v>
@@ -9314,31 +9375,31 @@
         <v>206</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="11" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="S19" s="11" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="T19" s="11" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="U19" s="11"/>
       <c r="V19" s="11"/>
       <c r="Y19" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="Z19" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="AA19" s="1" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="20" spans="1:27" ht="42">
@@ -9346,7 +9407,7 @@
         <v>487</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C20" s="3">
         <v>150</v>
@@ -9382,31 +9443,31 @@
         <v>247</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
       <c r="R20" s="11" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="S20" s="11" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="T20" s="11" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="U20" s="11"/>
       <c r="V20" s="11"/>
       <c r="Y20" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="Z20" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="AA20" s="1" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="21" spans="1:27" ht="42">
@@ -9414,7 +9475,7 @@
         <v>492</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C21" s="3">
         <v>100</v>
@@ -9450,31 +9511,31 @@
         <v>210</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
       <c r="R21" s="11" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="S21" s="11" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="T21" s="11" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="U21" s="11"/>
       <c r="V21" s="11"/>
       <c r="Y21" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="Z21" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="AA21" s="1" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="22" spans="1:27" ht="42">
@@ -9482,7 +9543,7 @@
         <v>492</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C22" s="3">
         <v>100</v>
@@ -9518,31 +9579,31 @@
         <v>166</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
       <c r="R22" s="11" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="S22" s="11" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="T22" s="11" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="U22" s="11"/>
       <c r="V22" s="11"/>
       <c r="Y22" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="Z22" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="AA22" s="1" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
     <row r="23" spans="1:27" ht="56">
@@ -9550,7 +9611,7 @@
         <v>555</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C23" s="3">
         <v>105</v>
@@ -9586,31 +9647,31 @@
         <v>114</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
       <c r="R23" s="11" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="S23" s="11" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="T23" s="11" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="U23" s="11"/>
       <c r="V23" s="11"/>
       <c r="Y23" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="Z23" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="AA23" s="1" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="24" spans="1:27" ht="42">
@@ -9618,7 +9679,7 @@
         <v>555</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C24" s="3">
         <v>105</v>
@@ -9654,31 +9715,31 @@
         <v>202</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
       <c r="R24" s="11" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="S24" s="11" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="T24" s="11" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="U24" s="11"/>
       <c r="V24" s="11"/>
       <c r="Y24" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="Z24" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="AA24" s="1" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="25" spans="1:27" ht="42">
@@ -9686,7 +9747,7 @@
         <v>641</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C25" s="3">
         <v>79</v>
@@ -9722,31 +9783,31 @@
         <v>169</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
       <c r="R25" s="11" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="S25" s="11" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="T25" s="11" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="U25" s="11"/>
       <c r="V25" s="11"/>
       <c r="Y25" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="Z25" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="AA25" s="1" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="26" spans="1:27" ht="42">
@@ -9754,7 +9815,7 @@
         <v>641</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C26" s="3">
         <v>79</v>
@@ -9790,31 +9851,31 @@
         <v>194</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
       <c r="R26" s="11" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="S26" s="11" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="T26" s="11" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="U26" s="11"/>
       <c r="V26" s="11"/>
       <c r="Y26" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="Z26" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="AA26" s="1" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="27" spans="1:27" ht="56">
@@ -9822,7 +9883,7 @@
         <v>642</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C27" s="3">
         <v>79</v>
@@ -9858,31 +9919,31 @@
         <v>169</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
       <c r="R27" s="11" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="S27" s="11" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="T27" s="11" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="U27" s="11"/>
       <c r="V27" s="11"/>
       <c r="Y27" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="Z27" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="AA27" s="1" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="28" spans="1:27" ht="42">
@@ -9890,7 +9951,7 @@
         <v>642</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C28" s="3">
         <v>79</v>
@@ -9926,31 +9987,31 @@
         <v>166</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
       <c r="R28" s="11" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="S28" s="11" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="T28" s="11" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="U28" s="11"/>
       <c r="V28" s="11"/>
       <c r="Y28" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="Z28" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="AA28" s="1" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="29" spans="1:27" ht="42">
@@ -9958,7 +10019,7 @@
         <v>645</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C29" s="3">
         <v>89</v>
@@ -9994,31 +10055,31 @@
         <v>187</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
       <c r="R29" s="11" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="S29" s="11" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="T29" s="11" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="U29" s="11"/>
       <c r="V29" s="11"/>
       <c r="Y29" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="Z29" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="AA29" s="1" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="30" spans="1:27" ht="42">
@@ -10026,7 +10087,7 @@
         <v>645</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C30" s="3">
         <v>89</v>
@@ -10062,31 +10123,31 @@
         <v>184</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
       <c r="R30" s="11" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="S30" s="11" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="T30" s="11" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="U30" s="11"/>
       <c r="V30" s="11"/>
       <c r="Y30" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="Z30" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="AA30" s="1" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="31" spans="1:27">
@@ -10094,7 +10155,7 @@
         <v>646</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C31" s="3">
         <v>125</v>
@@ -10130,29 +10191,29 @@
         <v>187</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
       <c r="R31" s="24" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="S31" s="24" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="T31" s="24" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="Y31" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="Z31" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="AA31" s="1" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="32" spans="1:27" ht="42">
@@ -10160,7 +10221,7 @@
         <v>646</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C32" s="17">
         <v>125</v>
@@ -10196,29 +10257,29 @@
         <v>206</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
       <c r="R32" s="11" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="S32" s="11" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="T32" s="11" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="Y32" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="Z32" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="AA32" s="1" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="33" spans="1:27" ht="42">
@@ -10226,7 +10287,7 @@
         <v>646</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C33" s="3">
         <v>125</v>
@@ -10262,29 +10323,29 @@
         <v>206</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
       <c r="R33" s="11" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="S33" s="11" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="T33" s="11" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="Y33" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="Z33" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="AA33" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="34" spans="1:27" ht="42">
@@ -10292,7 +10353,7 @@
         <v>648</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C34" s="3">
         <v>100</v>
@@ -10328,29 +10389,29 @@
         <v>250</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
       <c r="R34" s="24" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="S34" s="24" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="T34" s="24" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="Y34" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="Z34" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="AA34" s="1" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="35" spans="1:27" ht="42">
@@ -10358,7 +10419,7 @@
         <v>648</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C35" s="3">
         <v>100</v>
@@ -10394,29 +10455,29 @@
         <v>196</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
       <c r="R35" s="24" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="S35" s="24" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="T35" s="24" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="Y35" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="Z35" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="AA35" s="1" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="36" spans="1:27" ht="17">
@@ -10424,7 +10485,7 @@
         <v>658</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C36" s="25">
         <v>72</v>
@@ -10460,25 +10521,25 @@
         <v>154</v>
       </c>
       <c r="M36" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="R36" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="S36" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="T36" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="Y36" t="s">
         <v>184</v>
       </c>
-      <c r="R36" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="S36" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="T36" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="Y36" t="s">
-        <v>188</v>
-      </c>
       <c r="Z36" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="AA36" s="1" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
     <row r="37" spans="1:27" ht="17">
@@ -10486,7 +10547,7 @@
         <v>658</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C37" s="25">
         <v>72</v>
@@ -10522,25 +10583,25 @@
         <v>157</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="R37" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="S37" s="11" t="s">
+        <v>382</v>
+      </c>
+      <c r="T37" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="Y37" t="s">
+        <v>185</v>
+      </c>
+      <c r="Z37" t="s">
         <v>183</v>
       </c>
-      <c r="S37" s="11" t="s">
-        <v>386</v>
-      </c>
-      <c r="T37" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="Y37" t="s">
-        <v>189</v>
-      </c>
-      <c r="Z37" t="s">
-        <v>187</v>
-      </c>
       <c r="AA37" s="1" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="38" spans="1:27" ht="42">
@@ -10548,7 +10609,7 @@
         <v>681</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C38" s="3">
         <v>60</v>
@@ -10584,31 +10645,31 @@
         <v>291</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
       <c r="Q38" s="25"/>
       <c r="R38" s="11" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="S38" s="11" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="T38" s="11" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="U38" s="11"/>
       <c r="V38" s="11"/>
       <c r="Y38" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="Z38" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="AA38" s="1" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="39" spans="1:27" ht="43" thickBot="1">
@@ -10616,7 +10677,7 @@
         <v>681</v>
       </c>
       <c r="B39" s="27" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C39" s="28">
         <v>60</v>
@@ -10652,28 +10713,28 @@
         <v>97</v>
       </c>
       <c r="M39" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="Q39" s="25"/>
       <c r="R39" s="11" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="S39" s="11" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="T39" s="11" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="U39" s="11"/>
       <c r="V39" s="11"/>
       <c r="Y39" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="Z39" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="AA39" s="1" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="40" spans="1:27" ht="43" thickTop="1">
@@ -10681,7 +10742,7 @@
         <v>710</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C40" s="3">
         <v>59</v>
@@ -10717,29 +10778,29 @@
         <v>127</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
       <c r="Q40" s="25"/>
       <c r="R40" s="11" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="S40" s="11" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="T40" s="11" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="Y40" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="Z40" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="AA40" s="1" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="41" spans="1:27" ht="42">
@@ -10747,7 +10808,7 @@
         <v>710</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C41" s="3">
         <v>54</v>
@@ -10783,29 +10844,29 @@
         <v>128</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="N41" s="1"/>
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
       <c r="Q41" s="25"/>
       <c r="R41" s="11" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="S41" s="11" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="T41" s="11" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="Y41" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="Z41" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="AA41" s="1" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="42" spans="1:27" ht="42">
@@ -10813,7 +10874,7 @@
         <v>710</v>
       </c>
       <c r="B42" s="15" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C42" s="3">
         <v>49</v>
@@ -10849,29 +10910,29 @@
         <v>129</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="N42" s="1"/>
       <c r="O42" s="1"/>
       <c r="P42" s="1"/>
       <c r="Q42" s="25"/>
       <c r="R42" s="11" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="S42" s="11" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="T42" s="11" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="Y42" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="Z42" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="AA42" s="1" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="43" spans="1:27" ht="42">
@@ -10879,7 +10940,7 @@
         <v>710</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C43" s="3">
         <v>44</v>
@@ -10915,29 +10976,29 @@
         <v>131</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="N43" s="1"/>
       <c r="O43" s="1"/>
       <c r="P43" s="1"/>
       <c r="Q43" s="25"/>
       <c r="R43" s="11" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="S43" s="11" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="T43" s="11" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="Y43" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="Z43" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="AA43" s="1" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="44" spans="1:27" ht="42">
@@ -10945,7 +11006,7 @@
         <v>711</v>
       </c>
       <c r="B44" s="15" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C44" s="3">
         <v>85</v>
@@ -10981,29 +11042,29 @@
         <v>222</v>
       </c>
       <c r="M44" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="N44" s="1"/>
       <c r="O44" s="1"/>
       <c r="P44" s="1"/>
       <c r="Q44" s="25"/>
       <c r="R44" s="11" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="S44" s="11" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="T44" s="11" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="Y44" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="Z44" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="AA44" s="1" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="45" spans="1:27" ht="42">
@@ -11011,7 +11072,7 @@
         <v>711</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C45" s="3">
         <v>75</v>
@@ -11047,29 +11108,29 @@
         <v>229</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="N45" s="1"/>
       <c r="O45" s="1"/>
       <c r="P45" s="1"/>
       <c r="Q45" s="25"/>
       <c r="R45" s="11" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="S45" s="11" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="T45" s="11" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="Y45" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="Z45" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="AA45" s="1" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="46" spans="1:27" ht="42">
@@ -11077,7 +11138,7 @@
         <v>711</v>
       </c>
       <c r="B46" s="15" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C46" s="3">
         <v>65</v>
@@ -11113,29 +11174,29 @@
         <v>236</v>
       </c>
       <c r="M46" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="N46" s="1"/>
       <c r="O46" s="1"/>
       <c r="P46" s="1"/>
       <c r="Q46" s="25"/>
       <c r="R46" s="11" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="S46" s="11" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="T46" s="11" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="Y46" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="Z46" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="AA46" s="1" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="47" spans="1:27" ht="42">
@@ -11143,7 +11204,7 @@
         <v>711</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C47" s="3">
         <v>55</v>
@@ -11179,29 +11240,29 @@
         <v>243</v>
       </c>
       <c r="M47" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="N47" s="1"/>
       <c r="O47" s="1"/>
       <c r="P47" s="1"/>
       <c r="Q47" s="25"/>
       <c r="R47" s="11" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="S47" s="11" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="T47" s="11" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="Y47" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="Z47" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="AA47" s="1" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="48" spans="1:27" ht="42">
@@ -11209,7 +11270,7 @@
         <v>718</v>
       </c>
       <c r="B48" s="15" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C48" s="3">
         <v>108</v>
@@ -11245,31 +11306,31 @@
         <v>245</v>
       </c>
       <c r="M48" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="N48" s="1"/>
       <c r="O48" s="1"/>
       <c r="P48" s="1"/>
       <c r="Q48" s="1"/>
       <c r="R48" s="11" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="S48" s="11" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="T48" s="11" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="U48" s="1"/>
       <c r="W48" s="1"/>
       <c r="Y48" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="Z48" s="35" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="AA48" s="35" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="49" spans="1:27" ht="42">
@@ -11277,7 +11338,7 @@
         <v>718</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C49" s="3">
         <v>54</v>
@@ -11313,31 +11374,31 @@
         <v>180</v>
       </c>
       <c r="M49" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="N49" s="1"/>
       <c r="O49" s="1"/>
       <c r="P49" s="1"/>
       <c r="Q49" s="1"/>
       <c r="R49" s="11" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="S49" s="11" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="T49" s="11" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="U49" s="1"/>
       <c r="W49" s="1"/>
       <c r="Y49" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="Z49" s="35" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="AA49" s="35" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="50" spans="1:27" ht="42">
@@ -11345,7 +11406,7 @@
         <v>718</v>
       </c>
       <c r="B50" s="15" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C50" s="3">
         <v>216</v>
@@ -11381,31 +11442,31 @@
         <v>241</v>
       </c>
       <c r="M50" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="N50" s="1"/>
       <c r="O50" s="1"/>
       <c r="P50" s="1"/>
       <c r="Q50" s="1"/>
       <c r="R50" s="11" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="S50" s="11" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="T50" s="11" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="U50" s="1"/>
       <c r="W50" s="1"/>
       <c r="Y50" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="Z50" s="35" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="AA50" s="35" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="51" spans="1:27" ht="42">
@@ -11413,7 +11474,7 @@
         <v>720</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C51" s="3">
         <v>80</v>
@@ -11449,31 +11510,31 @@
         <v>241</v>
       </c>
       <c r="M51" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="N51" s="1"/>
       <c r="O51" s="1"/>
       <c r="P51" s="1"/>
       <c r="Q51" s="1"/>
       <c r="R51" s="11" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="S51" s="11" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="T51" s="11" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="U51" s="11"/>
       <c r="V51" s="11"/>
       <c r="Y51" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="Z51" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="AA51" s="35" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="52" spans="1:27" ht="42">
@@ -11481,7 +11542,7 @@
         <v>720</v>
       </c>
       <c r="B52" s="15" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C52" s="3">
         <v>80</v>
@@ -11517,31 +11578,31 @@
         <v>245</v>
       </c>
       <c r="M52" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="N52" s="1"/>
       <c r="O52" s="1"/>
       <c r="P52" s="1"/>
       <c r="Q52" s="1"/>
       <c r="R52" s="11" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="S52" s="11" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="T52" s="11" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="U52" s="11"/>
       <c r="V52" s="11"/>
       <c r="Y52" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="Z52" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="AA52" s="35" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="53" spans="1:27" ht="25">
@@ -11549,7 +11610,7 @@
         <v>741</v>
       </c>
       <c r="B53" s="36" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="C53" s="43">
         <v>75</v>
@@ -11586,29 +11647,29 @@
         <v>145</v>
       </c>
       <c r="M53" s="1" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="N53" s="1"/>
       <c r="O53" s="1"/>
       <c r="P53" s="1"/>
       <c r="Q53" s="1"/>
       <c r="R53" s="11" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="S53" s="11" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="T53" s="11" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="Y53" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="Z53" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="AA53" s="35" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="54" spans="1:27" ht="37">
@@ -11616,7 +11677,7 @@
         <v>741</v>
       </c>
       <c r="B54" s="36" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="C54" s="43">
         <v>75</v>
@@ -11653,29 +11714,29 @@
         <v>145</v>
       </c>
       <c r="M54" s="1" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="N54" s="1"/>
       <c r="O54" s="1"/>
       <c r="P54" s="1"/>
       <c r="Q54" s="1"/>
       <c r="R54" s="11" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="S54" s="11" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="T54" s="11" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="Y54" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="Z54" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="AA54" s="35" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
     </row>
     <row r="55" spans="1:27" ht="25">
@@ -11683,7 +11744,7 @@
         <v>741</v>
       </c>
       <c r="B55" s="36" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C55" s="43">
         <v>75</v>
@@ -11720,29 +11781,29 @@
         <v>145</v>
       </c>
       <c r="M55" s="1" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="N55" s="1"/>
       <c r="O55" s="1"/>
       <c r="P55" s="1"/>
       <c r="Q55" s="1"/>
       <c r="R55" s="11" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="S55" s="11" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="T55" s="11" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="Y55" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="Z55" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="AA55" s="35" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="56" spans="1:27" ht="37">
@@ -11750,7 +11811,7 @@
         <v>741</v>
       </c>
       <c r="B56" s="36" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C56" s="43">
         <v>75</v>
@@ -11787,29 +11848,29 @@
         <v>145</v>
       </c>
       <c r="M56" s="1" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="N56" s="1"/>
       <c r="O56" s="1"/>
       <c r="P56" s="1"/>
       <c r="Q56" s="1"/>
       <c r="R56" s="11" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="S56" s="11" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="T56" s="11" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="Y56" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="Z56" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="AA56" s="35" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
     <row r="57" spans="1:27" ht="37">
@@ -11817,7 +11878,7 @@
         <v>745</v>
       </c>
       <c r="B57" s="36" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="C57" s="37">
         <v>75</v>
@@ -11854,29 +11915,29 @@
         <v>140</v>
       </c>
       <c r="M57" s="1" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="N57" s="1"/>
       <c r="O57" s="1"/>
       <c r="P57" s="1"/>
       <c r="Q57" s="1"/>
       <c r="R57" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="S57" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="T57" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="Y57" t="s">
         <v>253</v>
       </c>
-      <c r="S57" s="11" t="s">
-        <v>253</v>
-      </c>
-      <c r="T57" s="11" t="s">
-        <v>253</v>
-      </c>
-      <c r="Y57" t="s">
-        <v>257</v>
-      </c>
       <c r="Z57" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="AA57" s="35" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="58" spans="1:27" ht="37">
@@ -11884,7 +11945,7 @@
         <v>745</v>
       </c>
       <c r="B58" s="36" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="C58" s="43">
         <v>85</v>
@@ -11921,29 +11982,29 @@
         <v>152</v>
       </c>
       <c r="M58" s="1" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="N58" s="1"/>
       <c r="O58" s="1"/>
       <c r="P58" s="1"/>
       <c r="Q58" s="1"/>
       <c r="R58" s="11" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="S58" s="11" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="T58" s="11" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="Y58" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="Z58" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="AA58" s="35" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
     </row>
     <row r="59" spans="1:27" ht="25">
@@ -11951,7 +12012,7 @@
         <v>745</v>
       </c>
       <c r="B59" s="36" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C59" s="37">
         <v>75</v>
@@ -11988,29 +12049,29 @@
         <v>139</v>
       </c>
       <c r="M59" s="1" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="N59" s="1"/>
       <c r="O59" s="1"/>
       <c r="P59" s="1"/>
       <c r="Q59" s="1"/>
       <c r="R59" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="S59" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="T59" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="Y59" t="s">
+        <v>260</v>
+      </c>
+      <c r="Z59" t="s">
         <v>256</v>
       </c>
-      <c r="S59" s="11" t="s">
-        <v>256</v>
-      </c>
-      <c r="T59" s="11" t="s">
-        <v>256</v>
-      </c>
-      <c r="Y59" t="s">
-        <v>264</v>
-      </c>
-      <c r="Z59" t="s">
-        <v>260</v>
-      </c>
       <c r="AA59" s="35" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="60" spans="1:27" ht="25">
@@ -12018,7 +12079,7 @@
         <v>746</v>
       </c>
       <c r="B60" s="36" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C60" s="43">
         <v>45</v>
@@ -12055,29 +12116,29 @@
         <v>46</v>
       </c>
       <c r="M60" s="1" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="N60" s="1"/>
       <c r="O60" s="1"/>
       <c r="P60" s="1"/>
       <c r="Q60" s="1"/>
       <c r="R60" s="11" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="S60" s="11" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="T60" s="11" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="Y60" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="Z60" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="AA60" s="35" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
     </row>
     <row r="61" spans="1:27" ht="25">
@@ -12085,7 +12146,7 @@
         <v>746</v>
       </c>
       <c r="B61" s="36" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="C61" s="43">
         <v>45</v>
@@ -12122,29 +12183,29 @@
         <v>245</v>
       </c>
       <c r="M61" s="1" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="N61" s="1"/>
       <c r="O61" s="1"/>
       <c r="P61" s="1"/>
       <c r="Q61" s="1"/>
       <c r="R61" s="11" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="S61" s="11" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="T61" s="11" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="Y61" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="Z61" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="AA61" s="35" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="62" spans="1:27" ht="37">
@@ -12152,7 +12213,7 @@
         <v>774</v>
       </c>
       <c r="B62" s="36" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="C62" s="43">
         <v>60</v>
@@ -12189,29 +12250,29 @@
         <v>194</v>
       </c>
       <c r="M62" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="N62" s="1"/>
       <c r="O62" s="1"/>
       <c r="P62" s="1"/>
       <c r="Q62" s="1"/>
       <c r="R62" s="11" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="S62" s="11" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="T62" s="11" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="Y62" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="Z62" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="AA62" s="35" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
     <row r="63" spans="1:27" ht="25">
@@ -12219,7 +12280,7 @@
         <v>774</v>
       </c>
       <c r="B63" s="36" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C63" s="43">
         <v>60</v>
@@ -12256,29 +12317,29 @@
         <v>131</v>
       </c>
       <c r="M63" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="N63" s="1"/>
       <c r="O63" s="1"/>
       <c r="P63" s="1"/>
       <c r="Q63" s="1"/>
       <c r="R63" s="11" t="s">
+        <v>265</v>
+      </c>
+      <c r="S63" s="11" t="s">
+        <v>265</v>
+      </c>
+      <c r="T63" s="11" t="s">
+        <v>265</v>
+      </c>
+      <c r="Y63" t="s">
         <v>269</v>
       </c>
-      <c r="S63" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="T63" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="Y63" t="s">
-        <v>273</v>
-      </c>
       <c r="Z63" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="AA63" s="35" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="64" spans="1:27">
@@ -12286,7 +12347,7 @@
         <v>800</v>
       </c>
       <c r="B64" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C64" s="43">
         <v>97</v>
@@ -12323,29 +12384,29 @@
         <v>201</v>
       </c>
       <c r="M64" s="1" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="N64" s="1"/>
       <c r="O64" s="1"/>
       <c r="P64" s="1"/>
       <c r="Q64" s="1"/>
       <c r="R64" s="11" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="S64" s="11" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="T64" s="11" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="Y64" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="Z64" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="AA64" s="35" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="65" spans="1:27" ht="25">
@@ -12353,7 +12414,7 @@
         <v>800</v>
       </c>
       <c r="B65" s="36" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="C65" s="43">
         <v>97</v>
@@ -12390,29 +12451,29 @@
         <v>251</v>
       </c>
       <c r="M65" s="1" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="N65" s="1"/>
       <c r="O65" s="1"/>
       <c r="P65" s="1"/>
       <c r="Q65" s="1"/>
       <c r="R65" s="11" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="S65" s="11" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="T65" s="11" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="Y65" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="Z65" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="AA65" s="35" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="66" spans="1:27">
@@ -12420,7 +12481,7 @@
         <v>800</v>
       </c>
       <c r="B66" s="45" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="C66" s="43">
         <v>97</v>
@@ -12457,29 +12518,29 @@
         <v>251</v>
       </c>
       <c r="M66" s="1" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="N66" s="1"/>
       <c r="O66" s="1"/>
       <c r="P66" s="1"/>
       <c r="Q66" s="1"/>
       <c r="R66" s="11" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="S66" s="11" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="T66" s="11" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="Y66" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="Z66" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="AA66" s="35" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="67" spans="1:27">
@@ -12487,7 +12548,7 @@
         <v>800</v>
       </c>
       <c r="B67" s="45" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C67" s="43">
         <v>97</v>
@@ -12524,29 +12585,29 @@
         <v>215</v>
       </c>
       <c r="M67" s="1" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="N67" s="1"/>
       <c r="O67" s="1"/>
       <c r="P67" s="1"/>
       <c r="Q67" s="1"/>
       <c r="R67" s="11" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="S67" s="11" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="T67" s="11" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="Y67" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="Z67" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="AA67" s="35" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add nerf (over 4k), rotom (mow) modified, add exclusive moves to pikachu & dragonite
</commit_message>
<xml_diff>
--- a/form_diff.xlsx
+++ b/form_diff.xlsx
@@ -8007,8 +8007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -9277,19 +9277,19 @@
         <v>50</v>
       </c>
       <c r="D18" s="4">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="E18" s="5">
-        <v>77</v>
+        <v>107</v>
       </c>
       <c r="F18" s="6">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="G18" s="7">
-        <v>77</v>
+        <v>107</v>
       </c>
       <c r="H18" s="8">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="I18" s="9">
         <v>440</v>
@@ -9300,11 +9300,11 @@
       </c>
       <c r="K18" s="1">
         <f t="shared" si="1"/>
-        <v>185</v>
+        <v>204</v>
       </c>
       <c r="L18" s="1">
         <f t="shared" si="2"/>
-        <v>159</v>
+        <v>219</v>
       </c>
       <c r="M18" s="1" t="s">
         <v>83</v>

</xml_diff>